<commit_message>
added the answer pdf
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -19,19 +19,19 @@
     <t>1</t>
   </si>
   <si>
-    <t>How are you?</t>
+    <t>WHAT IS MACHINE LEARNING?</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>What is your age ?</t>
+    <t>What are the main types of machine learning algorithms ?</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>What do you study</t>
+    <t>Explain the concept of machine learning.</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>